<commit_message>
final push for clue board part 1.
</commit_message>
<xml_diff>
--- a/ourData/ClueLayout.xlsx
+++ b/ourData/ClueLayout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueLayout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGameBSJM\ourData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,71 +2047,69 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2">
         <v>0</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
       <c r="C23" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2">
         <v>5</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>6</v>
       </c>
-      <c r="H23" s="2">
-        <v>7</v>
-      </c>
       <c r="I23" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J23" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K23" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L23" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M23" s="2">
+        <v>11</v>
+      </c>
+      <c r="N23" s="2">
         <v>12</v>
       </c>
-      <c r="N23" s="2">
+      <c r="O23" s="2">
         <v>13</v>
       </c>
-      <c r="O23" s="2">
+      <c r="P23" s="2">
         <v>14</v>
       </c>
-      <c r="P23" s="2">
+      <c r="Q23" s="2">
         <v>15</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="R23" s="2">
         <v>16</v>
       </c>
-      <c r="R23" s="2">
+      <c r="S23" s="2">
         <v>17</v>
       </c>
-      <c r="S23" s="2">
+      <c r="T23" s="2">
         <v>18</v>
       </c>
-      <c r="T23" s="2">
+      <c r="U23" s="2">
         <v>19</v>
       </c>
-      <c r="U23" s="2">
+      <c r="V23" s="2">
         <v>20</v>
-      </c>
-      <c r="V23" s="2">
-        <v>21</v>
       </c>
       <c r="W23" s="3"/>
     </row>

</xml_diff>